<commit_message>
adding groups to the app, each Filiere has one or many groups
</commit_message>
<xml_diff>
--- a/app/resources/canvas/stagiaire-canva.xlsx
+++ b/app/resources/canvas/stagiaire-canva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ABS-ISTA\app\resources\canvas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93C73F6-4ECD-4D73-BDCC-D9692FDA01F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E17DEF-82D7-45A1-B74B-88F67609744B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Filiere</t>
+    <t>Groupe</t>
   </si>
 </sst>
 </file>
@@ -102,7 +102,7 @@
     <tableColumn id="2" xr3:uid="{C283FC8E-1F74-4298-88D9-3C355A7895A7}" name="Nom"/>
     <tableColumn id="3" xr3:uid="{24586F87-24B4-437D-88C6-8607AD59071D}" name="Email"/>
     <tableColumn id="4" xr3:uid="{BFBA7DFE-1E9B-429F-BFB2-2A2A94112D43}" name="Numero de telephone"/>
-    <tableColumn id="5" xr3:uid="{F1340D97-6FFE-40F1-A88D-97ABD58ACBEA}" name="Filiere"/>
+    <tableColumn id="5" xr3:uid="{F1340D97-6FFE-40F1-A88D-97ABD58ACBEA}" name="Groupe"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -374,7 +374,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>